<commit_message>
Separated master notebook into individual notebooks - added read me file with model comments
</commit_message>
<xml_diff>
--- a/BLM WY 3-24-20 Sale/Output Data/Sale Tracts Learning Measures.xlsx
+++ b/BLM WY 3-24-20 Sale/Output Data/Sale Tracts Learning Measures.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -418,75 +418,55 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Permit Summary</t>
+          <t>Record Date</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Recent Prod Summary</t>
+          <t>Total Permits</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Leases Summary</t>
+          <t>Total Wells</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Old Production Summary</t>
+          <t>Avg First 6 Mo Oil</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Record Date</t>
+          <t>Avg First 6 Mo Gas</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Total Permits</t>
+          <t>Qi Oil</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Total Wells</t>
+          <t>Qi Gas</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Avg First 6 Mo Oil</t>
+          <t>6 Mo Oil Revenue $</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Avg First 6 Mo Gas</t>
+          <t>6 Mo Gas Rev $</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Qi Oil</t>
+          <t>Oil Price</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Qi Gas</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>6 Mo Oil Revenue $</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>6 Mo Gas Rev $</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Oil Price</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Gas Price</t>
         </is>
@@ -535,65 +515,37 @@
           <t>POLYGON ((474786.293277905 4783844.910772996, 474771.4101035152 4783466.10868964, 474726.8523400651 4783089.642047092, 474652.8947009834 4782717.831887392, 474549.9931597083 4782352.970543814, 474418.7821384601 4781997.307507869, 474260.0705968169 4781653.035560443, 474074.8370442098 4781322.277252576, 473864.2235070871 4781007.071819223, 473629.5284879412 4780709.362606697, 473372.1989596093 4780430.985091291, 473093.8214442041 4780173.65556296, 472796.112231678 4779938.960543814, 472480.9067983248 4779728.347006692, 472150.1484904575 4779543.113454084, 471805.8765430322 4779384.401912441, 471450.2135070871 4779253.190891192, 471085.3521635085 4779150.289349917, 470713.5420038085 4779076.331710836, 470337.0753612609 4779031.773947386, 469958.273277905 4779016.890772996, 469579.471194549 4779031.773947386, 469203.0045520014 4779076.331710836, 468831.1943923014 4779150.289349917, 468466.3330487228 4779253.190891192, 468110.6700127777 4779384.401912441, 467766.3980653525 4779543.113454084, 467435.6397574851 4779728.347006692, 467120.4343241319 4779938.960543814, 466822.7251116059 4780173.65556296, 466544.3475962007 4780430.985091291, 466287.0180678687 4780709.362606697, 466052.3230487228 4781007.071819223, 465841.7095116001 4781322.277252576, 465656.475958993 4781653.035560443, 465497.7644173498 4781997.307507869, 465366.5533961016 4782352.970543814, 465263.6518548265 4782717.831887392, 465189.6942157448 4783089.642047092, 465145.1364522947 4783466.10868964, 465130.2532779049 4783844.910772996, 465145.1364522947 4784223.712856352, 465189.6942157448 4784600.1794989, 465263.6518548265 4784971.9896586, 465366.5533961016 4785336.851002178, 465497.7644173498 4785692.514038123, 465656.475958993 4786036.785985549, 465841.7095116001 4786367.544293416, 466052.3230487228 4786682.74972677, 466287.0180678687 4786980.458939295, 466544.3475962006 4787258.836454701, 466822.7251116058 4787516.165983032, 467120.4343241318 4787750.861002178, 467435.6397574851 4787961.4745393, 467766.3980653524 4788146.708091908, 468110.6700127776 4788305.419633552, 468466.3330487228 4788436.6306548, 468831.1943923014 4788539.532196075, 469203.0045520014 4788613.489835156, 469579.471194549 4788658.047598606, 469958.273277905 4788672.930772996, 470337.0753612609 4788658.047598606, 470713.5420038085 4788613.489835156, 471085.3521635085 4788539.532196075, 471450.213507087 4788436.6306548, 471805.8765430322 4788305.419633552, 472150.1484904574 4788146.708091908, 472480.9067983248 4787961.4745393, 472796.112231678 4787750.861002178, 473093.821444204 4787516.165983032, 473372.1989596092 4787258.836454701, 473629.5284879412 4786980.458939295, 473864.223507087 4786682.74972677, 474074.8370442098 4786367.544293416, 474260.0705968168 4786036.785985549, 474418.7821384601 4785692.514038123, 474549.9931597083 4785336.851002178, 474652.8947009833 4784971.9896586, 474726.8523400651 4784600.1794989, 474771.4101035151 4784223.712856352, 474786.293277905 4783844.910772996))</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 12 active permits
-8 permits are H wells ; 4 permits are V wells 
-The average lateral length among these permits is 9000 ft. 
-- The TVD for these well(s) are ~10500ft
-Devon has 12 permits</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 6 wells within 3 mile radius that have started producing within last 4 years
-6 are H wells
-1 well has made 68 mbbl and 92 mmcfd in 5 months and is currently making 306 bpd and 608 mcfd.  2 wells have produced for 6 to 8 months and have made between 82 to 145 mbbls with 47 to 86 mmcf of gas.  These wells are currently averaging 345 bpd and 276 mcfd.  1 well has made 198 mbbl and 236 mmcfd in 16 months and is currently making 234 bpd and 273 mcfd.  1 well has made 238 mbbl and 287 mmcfd in 22 months and is currently making 165 bpd and 164 mcfd.  1 well has made 214 mbbl and 119 mmcfd in 26 months and is currently making 194 bpd and 99 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2014.
-Mbi O&amp;G paid $3100/acre.  
-</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O2" s="2" t="n">
+      <c r="K2" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L2" t="n">
+        <v>12</v>
+      </c>
+      <c r="M2" t="n">
+        <v>6</v>
+      </c>
+      <c r="N2" t="n">
+        <v>107657.2</v>
+      </c>
+      <c r="O2" t="n">
+        <v>85665</v>
+      </c>
       <c r="P2" t="n">
-        <v>12</v>
+        <v>26755</v>
       </c>
       <c r="Q2" t="n">
-        <v>6</v>
+        <v>20090</v>
       </c>
       <c r="R2" t="n">
-        <v>107657.2</v>
+        <v>2691430</v>
       </c>
       <c r="S2" t="n">
-        <v>85665</v>
+        <v>153340.35</v>
       </c>
       <c r="T2" t="n">
-        <v>26755</v>
+        <v>25</v>
       </c>
       <c r="U2" t="n">
-        <v>20090</v>
-      </c>
-      <c r="V2" t="n">
-        <v>2691430</v>
-      </c>
-      <c r="W2" t="n">
-        <v>153340.35</v>
-      </c>
-      <c r="X2" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y2" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -640,65 +592,37 @@
           <t>POLYGON ((474781.1718195324 4784853.058404164, 474766.2886451426 4784474.256320808, 474721.7308816926 4784097.789678261, 474647.7732426108 4783725.979518561, 474544.8717013357 4783361.118174982, 474413.6606800875 4783005.455139037, 474254.9491384443 4782661.183191611, 474069.7155858373 4782330.424883745, 473859.1020487145 4782015.219450391, 473624.4070295686 4781717.510237865, 473367.0775012367 4781439.13272246, 473088.6999858315 4781181.803194128, 472790.9907733055 4780947.108174982, 472475.7853399523 4780736.49463786, 472145.0270320849 4780551.261085252, 471800.7550846597 4780392.549543609, 471445.0920487145 4780261.338522361, 471080.230705136 4780158.436981086, 470708.4205454359 4780084.479342004, 470331.9539028883 4780039.921578554, 469953.1518195324 4780025.038404165, 469574.3497361764 4780039.921578554, 469197.8830936289 4780084.479342004, 468826.0729339288 4780158.436981086, 468461.2115903503 4780261.338522361, 468105.5485544051 4780392.549543609, 467761.2766069799 4780551.261085252, 467430.5182991125 4780736.49463786, 467115.3128657593 4780947.108174982, 466817.6036532333 4781181.803194128, 466539.2261378281 4781439.13272246, 466281.8966094962 4781717.510237865, 466047.2015903502 4782015.219450391, 465836.5880532275 4782330.424883745, 465651.3545006205 4782661.183191611, 465492.6429589773 4783005.455139037, 465361.4319377291 4783361.118174982, 465258.530396454 4783725.979518561, 465184.5727573722 4784097.789678261, 465140.0149939221 4784474.256320808, 465125.1318195324 4784853.058404164, 465140.0149939221 4785231.860487521, 465184.5727573722 4785608.327130068, 465258.530396454 4785980.137289768, 465361.4319377291 4786344.998633347, 465492.6429589773 4786700.661669292, 465651.3545006205 4787044.933616717, 465836.5880532275 4787375.691924584, 466047.2015903502 4787690.897357938, 466281.8966094962 4787988.606570464, 466539.2261378281 4788266.984085869, 466817.6036532333 4788524.313614201, 467115.3128657592 4788759.008633346, 467430.5182991125 4788969.622170469, 467761.2766069798 4789154.855723076, 468105.548554405 4789313.56726472, 468461.2115903503 4789444.778285968, 468826.0729339288 4789547.679827243, 469197.8830936289 4789621.637466324, 469574.3497361764 4789666.195229774, 469953.1518195324 4789681.078404164, 470331.9539028883 4789666.195229774, 470708.4205454359 4789621.637466324, 471080.230705136 4789547.679827243, 471445.0920487145 4789444.778285968, 471800.7550846597 4789313.56726472, 472145.0270320849 4789154.855723076, 472475.7853399523 4788969.622170469, 472790.9907733055 4788759.008633346, 473088.6999858315 4788524.313614201, 473367.0775012366 4788266.984085869, 473624.4070295686 4787988.606570464, 473859.1020487145 4787690.897357938, 474069.7155858372 4787375.691924584, 474254.9491384443 4787044.933616717, 474413.6606800875 4786700.661669292, 474544.8717013357 4786344.998633347, 474647.7732426107 4785980.137289768, 474721.7308816925 4785608.327130068, 474766.2886451426 4785231.860487521, 474781.1718195324 4784853.058404164))</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 10 active permits
-6 permits are H wells ; 4 permits are V wells 
-The average lateral length among these permits is 9000 ft. 
-- The TVD for these well(s) are ~10300ft
-Devon has 10 permits</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 5 wells within 3 mile radius that have started producing within last 4 years
-5 are H wells
-2 wells have produced for 6 to 8 months and have made between 82 to 145 mbbls with 47 to 86 mmcf of gas.  These wells are currently averaging 345 bpd and 276 mcfd.  1 well has made 198 mbbl and 236 mmcfd in 16 months and is currently making 234 bpd and 273 mcfd.  1 well has made 238 mbbl and 287 mmcfd in 22 months and is currently making 165 bpd and 164 mcfd.  1 well has made 214 mbbl and 119 mmcfd in 26 months and is currently making 194 bpd and 99 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2014.
-Mbi O&amp;G paid $3100/acre.  
-</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O3" s="2" t="n">
+      <c r="K3" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L3" t="n">
+        <v>10</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N3" t="n">
+        <v>107657.2</v>
+      </c>
+      <c r="O3" t="n">
+        <v>85665</v>
+      </c>
       <c r="P3" t="n">
-        <v>10</v>
+        <v>27732</v>
       </c>
       <c r="Q3" t="n">
-        <v>5</v>
+        <v>18996</v>
       </c>
       <c r="R3" t="n">
-        <v>107657.2</v>
+        <v>2691430</v>
       </c>
       <c r="S3" t="n">
-        <v>85665</v>
+        <v>153340.35</v>
       </c>
       <c r="T3" t="n">
-        <v>27732</v>
+        <v>25</v>
       </c>
       <c r="U3" t="n">
-        <v>18996</v>
-      </c>
-      <c r="V3" t="n">
-        <v>2691430</v>
-      </c>
-      <c r="W3" t="n">
-        <v>153340.35</v>
-      </c>
-      <c r="X3" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y3" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -745,66 +669,37 @@
           <t>POLYGON ((472585.150082407 4784036.616042774, 472570.2669080172 4783657.813959418, 472525.7091445671 4783281.34731687, 472451.7515054854 4782909.53715717, 472348.8499642103 4782544.675813592, 472217.6389429621 4782189.012777647, 472058.9274013189 4781844.740830221, 471873.6938487118 4781513.982522354, 471663.0803115891 4781198.777089001, 471428.3852924432 4780901.067876475, 471171.0557641113 4780622.69036107, 470892.6782487061 4780365.360832738, 470594.9690361801 4780130.665813592, 470279.7636028269 4779920.05227647, 469949.0052949595 4779734.818723862, 469604.7333475343 4779576.107182219, 469249.0703115891 4779444.89616097, 468884.2089680106 4779341.994619695, 468512.3988083105 4779268.036980614, 468135.9321657629 4779223.479217164, 467757.130082407 4779208.596042775, 467378.327999051 4779223.479217164, 467001.8613565034 4779268.036980614, 466630.0511968034 4779341.994619695, 466265.1898532248 4779444.89616097, 465909.5268172797 4779576.107182219, 465565.2548698545 4779734.818723862, 465234.4965619871 4779920.05227647, 464919.2911286339 4780130.665813592, 464621.5819161079 4780365.360832738, 464343.2044007027 4780622.69036107, 464085.8748723707 4780901.067876475, 463851.1798532248 4781198.777089001, 463640.5663161022 4781513.982522354, 463455.332763495 4781844.740830221, 463296.6212218518 4782189.012777647, 463165.4102006037 4782544.675813592, 463062.5086593286 4782909.53715717, 462988.5510202468 4783281.34731687, 462943.9932567967 4783657.813959418, 462929.110082407 4784036.616042774, 462943.9932567967 4784415.41812613, 462988.5510202468 4784791.884768678, 463062.5086593286 4785163.694928378, 463165.4102006037 4785528.556271956, 463296.6212218518 4785884.219307901, 463455.332763495 4786228.491255327, 463640.5663161021 4786559.249563194, 463851.1798532248 4786874.454996548, 464085.8748723707 4787172.164209073, 464343.2044007027 4787450.541724479, 464621.5819161079 4787707.871252811, 464919.2911286338 4787942.566271956, 465234.4965619871 4788153.179809079, 465565.2548698544 4788338.413361686, 465909.5268172796 4788497.12490333, 466265.1898532248 4788628.335924578, 466630.0511968034 4788731.237465853, 467001.8613565034 4788805.195104934, 467378.327999051 4788849.752868384, 467757.130082407 4788864.636042774, 468135.9321657629 4788849.752868384, 468512.3988083105 4788805.195104934, 468884.2089680106 4788731.237465853, 469249.0703115891 4788628.335924578, 469604.7333475343 4788497.12490333, 469949.0052949595 4788338.413361686, 470279.7636028269 4788153.179809079, 470594.9690361801 4787942.566271956, 470892.678248706 4787707.871252811, 471171.0557641112 4787450.541724479, 471428.3852924432 4787172.164209073, 471663.0803115891 4786874.454996548, 471873.6938487118 4786559.249563194, 472058.9274013189 4786228.491255327, 472217.6389429621 4785884.219307901, 472348.8499642103 4785528.556271956, 472451.7515054853 4785163.694928378, 472525.7091445671 4784791.884768678, 472570.2669080172 4784415.41812613, 472585.150082407 4784036.616042774))</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 13 active permits
-13 permits are H wells 
-The average lateral length among these permits is 10000 ft. 
-- The TVD for these well(s) are ~10300ft
-Devon has 13 permits</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 10 wells within 3 mile radius that have started producing within last 4 years
-10 are H wells
-1 well has made 68 mbbl and 92 mmcfd in 5 months and is currently making 306 bpd and 608 mcfd.  2 wells have produced for 6 to 8 months and have made between 82 to 145 mbbls with 47 to 86 mmcf of gas.  These wells are currently averaging 345 bpd and 276 mcfd.  1 well has made 282 mbbl and 147 mmcfd in 12 months and is currently making 376 bpd and 174 mcfd.  1 well has made 198 mbbl and 236 mmcfd in 16 months and is currently making 234 bpd and 273 mcfd.  1 well has made 238 mbbl and 287 mmcfd in 22 months and is currently making 165 bpd and 164 mcfd.  1 well has made 214 mbbl and 119 mmcfd in 26 months and is currently making 194 bpd and 99 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Peak Powder River Resources paid $4002/acre.  
-In 2014, Mbi O&amp;G paid $3100/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O4" s="2" t="n">
+      <c r="K4" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L4" t="n">
+        <v>13</v>
+      </c>
+      <c r="M4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N4" t="n">
+        <v>122775</v>
+      </c>
+      <c r="O4" t="n">
+        <v>85716.83333333333</v>
+      </c>
       <c r="P4" t="n">
-        <v>13</v>
+        <v>27903</v>
       </c>
       <c r="Q4" t="n">
-        <v>10</v>
+        <v>18525</v>
       </c>
       <c r="R4" t="n">
-        <v>122775</v>
+        <v>3069375</v>
       </c>
       <c r="S4" t="n">
-        <v>85716.83333333333</v>
+        <v>153433.1316666667</v>
       </c>
       <c r="T4" t="n">
-        <v>27903</v>
+        <v>25</v>
       </c>
       <c r="U4" t="n">
-        <v>18525</v>
-      </c>
-      <c r="V4" t="n">
-        <v>3069375</v>
-      </c>
-      <c r="W4" t="n">
-        <v>153433.1316666667</v>
-      </c>
-      <c r="X4" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y4" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -851,65 +746,37 @@
           <t>POLYGON ((473660.8559083962 4802293.450434712, 473645.9727340065 4801914.648351355, 473601.4149705564 4801538.181708808, 473527.4573314746 4801166.371549108, 473424.5557901995 4800801.51020553, 473293.3447689514 4800445.847169585, 473134.6332273082 4800101.575222159, 472949.3996747011 4799770.816914292, 472738.7861375784 4799455.611480938, 472504.0911184325 4799157.902268413, 472246.7615901005 4798879.524753007, 471968.3840746954 4798622.195224675, 471670.6748621693 4798387.50020553, 471355.4694288161 4798176.886668407, 471024.7111209488 4797991.6531158, 470680.4391735235 4797832.941574156, 470324.7761375784 4797701.730552908, 469959.9147939998 4797598.829011633, 469588.1046342998 4797524.871372552, 469211.6379917522 4797480.313609102, 468832.8359083962 4797465.430434712, 468454.0338250403 4797480.313609102, 468077.5671824927 4797524.871372552, 467705.7570227926 4797598.829011633, 467340.8956792141 4797701.730552908, 466985.2326432689 4797832.941574156, 466640.9606958437 4797991.6531158, 466310.2023879763 4798176.886668407, 465994.9969546231 4798387.50020553, 465697.2877420972 4798622.195224675, 465418.910226692 4798879.524753007, 465161.58069836 4799157.902268413, 464926.8856792141 4799455.611480938, 464716.2721420914 4799770.816914292, 464531.0385894843 4800101.575222159, 464372.3270478411 4800445.847169585, 464241.1160265929 4800801.51020553, 464138.2144853178 4801166.371549108, 464064.2568462361 4801538.181708808, 464019.699082786 4801914.648351355, 464004.8159083962 4802293.450434712, 464019.699082786 4802672.252518068, 464064.2568462361 4803048.719160615, 464138.2144853178 4803420.529320315, 464241.1160265929 4803785.390663894, 464372.3270478411 4804141.053699839, 464531.0385894843 4804485.325647265, 464716.2721420914 4804816.083955131, 464926.8856792141 4805131.289388485, 465161.58069836 4805428.998601011, 465418.9102266919 4805707.376116416, 465697.2877420971 4805964.705644748, 465994.9969546231 4806199.400663894, 466310.2023879763 4806410.014201016, 466640.9606958437 4806595.247753624, 466985.2326432689 4806753.959295267, 467340.8956792141 4806885.170316515, 467705.7570227926 4806988.07185779, 468077.5671824927 4807062.029496872, 468454.0338250403 4807106.587260322, 468832.8359083962 4807121.470434711, 469211.6379917521 4807106.587260322, 469588.1046342998 4807062.029496872, 469959.9147939998 4806988.07185779, 470324.7761375783 4806885.170316515, 470680.4391735235 4806753.959295267, 471024.7111209487 4806595.247753624, 471355.4694288161 4806410.014201016, 471670.6748621693 4806199.400663894, 471968.3840746953 4805964.705644748, 472246.7615901005 4805707.376116416, 472504.0911184325 4805428.998601011, 472738.7861375783 4805131.289388485, 472949.399674701 4804816.083955131, 473134.6332273081 4804485.325647265, 473293.3447689514 4804141.053699839, 473424.5557901995 4803785.390663894, 473527.4573314746 4803420.529320315, 473601.4149705563 4803048.719160615, 473645.9727340064 4802672.252518068, 473660.8559083962 4802293.450434712))</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 11 active permits
-8 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 7000 ft. 
-- The TVD for these well(s) are ~10700ft
-Devon has 11 permits</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 15 wells within 3 mile radius that have started producing within last 4 years
-15 are H wells
-5 wells have produced for 2 to 3 months and have made between 22 to 50 mbbls with 20 to 83 mmcf of gas.  These wells are currently averaging 424 bpd and 628 mcfd.  4 wells have produced for 12 to 18 months and have made between 66 to 182 mbbls with 46 to 635 mmcf of gas.  These wells are currently averaging 64 bpd and 293 mcfd.  2 wells have produced for 19 to 24 months and have made between 72 to 101 mbbls with 69 to 160 mmcf of gas.  These wells are currently averaging 32 bpd and 59 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O5" s="2" t="n">
+      <c r="K5" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L5" t="n">
+        <v>11</v>
+      </c>
+      <c r="M5" t="n">
+        <v>15</v>
+      </c>
+      <c r="N5" t="n">
+        <v>84078.60000000001</v>
+      </c>
+      <c r="O5" t="n">
+        <v>136917.2</v>
+      </c>
       <c r="P5" t="n">
-        <v>11</v>
+        <v>19838</v>
       </c>
       <c r="Q5" t="n">
-        <v>15</v>
+        <v>32556</v>
       </c>
       <c r="R5" t="n">
-        <v>84078.60000000001</v>
+        <v>2101965</v>
       </c>
       <c r="S5" t="n">
-        <v>136917.2</v>
+        <v>245081.788</v>
       </c>
       <c r="T5" t="n">
-        <v>19838</v>
+        <v>25</v>
       </c>
       <c r="U5" t="n">
-        <v>32556</v>
-      </c>
-      <c r="V5" t="n">
-        <v>2101965</v>
-      </c>
-      <c r="W5" t="n">
-        <v>245081.788</v>
-      </c>
-      <c r="X5" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y5" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -956,66 +823,37 @@
           <t>POLYGON ((472436.491182364 4801534.516088142, 472421.6080079742 4801155.714004786, 472377.0502445241 4800779.247362238, 472303.0926054424 4800407.437202538, 472200.1910641673 4800042.57585896, 472068.9800429191 4799686.912823015, 471910.2685012759 4799342.640875589, 471725.0349486689 4799011.882567722, 471514.4214115461 4798696.677134369, 471279.7263924002 4798398.967921843, 471022.3968640683 4798120.590406437, 470744.0193486631 4797863.260878106, 470446.3101361371 4797628.56585896, 470131.1047027839 4797417.952321838, 469800.3463949165 4797232.71876923, 469456.0744474913 4797074.007227587, 469100.4114115461 4796942.796206338, 468735.5500679676 4796839.894665063, 468363.7399082675 4796765.937025982, 467987.2732657199 4796721.379262532, 467608.471182364 4796706.496088143, 467229.669099008 4796721.379262532, 466853.2024564605 4796765.937025982, 466481.3922967604 4796839.894665063, 466116.5309531818 4796942.796206338, 465760.8679172367 4797074.007227587, 465416.5959698115 4797232.71876923, 465085.8376619441 4797417.952321838, 464770.6322285909 4797628.56585896, 464472.9230160649 4797863.260878106, 464194.5455006597 4798120.590406437, 463937.2159723277 4798398.967921843, 463702.5209531818 4798696.677134369, 463491.9074160592 4799011.882567722, 463306.673863452 4799342.640875589, 463147.9623218089 4799686.912823015, 463016.7513005607 4800042.57585896, 462913.8497592856 4800407.437202538, 462839.8921202038 4800779.247362238, 462795.3343567537 4801155.714004786, 462780.451182364 4801534.516088142, 462795.3343567537 4801913.318171498, 462839.8921202038 4802289.784814046, 462913.8497592856 4802661.594973746, 463016.7513005607 4803026.456317324, 463147.9623218089 4803382.119353269, 463306.673863452 4803726.391300695, 463491.9074160591 4804057.149608562, 463702.5209531818 4804372.355041916, 463937.2159723277 4804670.064254441, 464194.5455006597 4804948.441769847, 464472.9230160649 4805205.771298178, 464770.6322285908 4805440.466317324, 465085.8376619441 4805651.079854446, 465416.5959698114 4805836.313407054, 465760.8679172366 4805995.024948698, 466116.5309531818 4806126.235969946, 466481.3922967604 4806229.137511221, 466853.2024564605 4806303.095150302, 467229.669099008 4806347.652913752, 467608.471182364 4806362.536088142, 467987.2732657199 4806347.652913752, 468363.7399082675 4806303.095150302, 468735.5500679676 4806229.137511221, 469100.4114115461 4806126.235969946, 469456.0744474913 4805995.024948698, 469800.3463949165 4805836.313407054, 470131.1047027839 4805651.079854446, 470446.3101361371 4805440.466317324, 470744.019348663 4805205.771298178, 471022.3968640682 4804948.441769847, 471279.7263924002 4804670.064254441, 471514.4214115461 4804372.355041916, 471725.0349486688 4804057.149608562, 471910.2685012759 4803726.391300695, 472068.9800429191 4803382.119353269, 472200.1910641673 4803026.456317324, 472303.0926054423 4802661.594973746, 472377.0502445241 4802289.784814046, 472421.6080079742 4801913.318171498, 472436.491182364 4801534.516088142))</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 20 active permits
-17 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 9000 ft. 
-- The TVD for these well(s) are ~10000ft
-Devon has 20 permits</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 22 wells within 3 mile radius that have started producing within last 4 years
-22 are H wells
-8 wells have produced for 2 to 3 months and have made between 22 to 85 mbbls with 20 to 92 mmcf of gas.  These wells are currently averaging 460 bpd and 723 mcfd.  2 wells have produced for 6 to 8 months and have made between 122 to 191 mbbls with 456 to 706 mmcf of gas.  These wells are currently averaging 385 bpd and 1973 mcfd.  6 wells have produced for 12 to 18 months and have made between 66 to 224 mbbls with 46 to 635 mmcf of gas.  These wells are currently averaging 44 bpd and 196 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-In 2014, Pacer Energy paid $3900/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O6" s="2" t="n">
+      <c r="K6" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L6" t="n">
+        <v>20</v>
+      </c>
+      <c r="M6" t="n">
+        <v>22</v>
+      </c>
+      <c r="N6" t="n">
+        <v>103078.4166666667</v>
+      </c>
+      <c r="O6" t="n">
+        <v>211061.5</v>
+      </c>
       <c r="P6" t="n">
-        <v>20</v>
+        <v>23465.45454545454</v>
       </c>
       <c r="Q6" t="n">
-        <v>22</v>
+        <v>38686.36363636363</v>
       </c>
       <c r="R6" t="n">
-        <v>103078.4166666667</v>
+        <v>2576960.416666667</v>
       </c>
       <c r="S6" t="n">
-        <v>211061.5</v>
+        <v>377800.085</v>
       </c>
       <c r="T6" t="n">
-        <v>23465.45454545454</v>
+        <v>25</v>
       </c>
       <c r="U6" t="n">
-        <v>38686.36363636363</v>
-      </c>
-      <c r="V6" t="n">
-        <v>2576960.416666667</v>
-      </c>
-      <c r="W6" t="n">
-        <v>377800.085</v>
-      </c>
-      <c r="X6" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y6" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -1062,65 +900,37 @@
           <t>POLYGON ((473718.6974940442 4801400.067115995, 473703.8143196544 4801021.265032639, 473659.2565562043 4800644.798390091, 473585.2989171226 4800272.988230391, 473482.3973758475 4799908.126886813, 473351.1863545993 4799552.463850868, 473192.4748129561 4799208.191903442, 473007.2412603491 4798877.433595575, 472796.6277232263 4798562.228162222, 472561.9327040804 4798264.518949696, 472304.6031757485 4797986.14143429, 472026.2256603433 4797728.811905959, 471728.5164478173 4797494.116886813, 471413.3110144641 4797283.503349691, 471082.5527065967 4797098.269797083, 470738.2807591715 4796939.55825544, 470382.6177232263 4796808.347234191, 470017.7563796478 4796705.445692916, 469645.9462199477 4796631.488053835, 469269.4795774001 4796586.930290385, 468890.6774940442 4796572.047115996, 468511.8754106882 4796586.930290385, 468135.4087681407 4796631.488053835, 467763.5986084406 4796705.445692916, 467398.7372648621 4796808.347234191, 467043.0742289169 4796939.55825544, 466698.8022814917 4797098.269797083, 466368.0439736243 4797283.503349691, 466052.8385402711 4797494.116886813, 465755.1293277451 4797728.811905959, 465476.7518123399 4797986.14143429, 465219.4222840079 4798264.518949696, 464984.727264862 4798562.228162222, 464774.1137277393 4798877.433595575, 464588.8801751322 4799208.191903442, 464430.1686334891 4799552.463850868, 464298.9576122409 4799908.126886813, 464196.0560709658 4800272.988230391, 464122.098431884 4800644.798390091, 464077.5406684339 4801021.265032639, 464062.6574940442 4801400.067115995, 464077.5406684339 4801778.869199351, 464122.098431884 4802155.335841899, 464196.0560709658 4802527.146001599, 464298.9576122409 4802892.007345177, 464430.1686334891 4803247.670381122, 464588.8801751322 4803591.942328548, 464774.1137277393 4803922.700636415, 464984.727264862 4804237.906069769, 465219.4222840079 4804535.615282294, 465476.7518123399 4804813.9927977, 465755.1293277451 4805071.322326032, 466052.838540271 4805306.017345177, 466368.0439736243 4805516.6308823, 466698.8022814916 4805701.864434907, 467043.0742289168 4805860.575976551, 467398.7372648621 4805991.786997799, 467763.5986084406 4806094.688539074, 468135.4087681407 4806168.646178155, 468511.8754106882 4806213.203941605, 468890.6774940442 4806228.087115995, 469269.4795774001 4806213.203941605, 469645.9462199477 4806168.646178155, 470017.7563796478 4806094.688539074, 470382.6177232263 4805991.786997799, 470738.2807591715 4805860.575976551, 471082.5527065967 4805701.864434907, 471413.3110144641 4805516.6308823, 471728.5164478173 4805306.017345177, 472026.2256603432 4805071.322326032, 472304.6031757484 4804813.9927977, 472561.9327040804 4804535.615282294, 472796.6277232263 4804237.906069769, 473007.241260349 4803922.700636415, 473192.4748129561 4803591.942328548, 473351.1863545993 4803247.670381122, 473482.3973758475 4802892.007345177, 473585.2989171225 4802527.146001599, 473659.2565562043 4802155.335841899, 473703.8143196544 4801778.869199351, 473718.6974940442 4801400.067115995))</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 11 active permits
-8 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 7000 ft. 
-- The TVD for these well(s) are ~10700ft
-Devon has 11 permits</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 13 wells within 3 mile radius that have started producing within last 4 years
-13 are H wells
-5 wells have produced for 2 to 3 months and have made between 22 to 50 mbbls with 20 to 83 mmcf of gas.  These wells are currently averaging 424 bpd and 628 mcfd.  2 wells have produced for 12 to 18 months and have made between 66 to 82 mbbls with 312 to 401 mmcf of gas.  These wells are currently averaging 64 bpd and 425 mcfd.  2 wells have produced for 19 to 24 months and have made between 72 to 101 mbbls with 69 to 160 mmcf of gas.  These wells are currently averaging 32 bpd and 59 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O7" s="2" t="n">
+      <c r="K7" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L7" t="n">
+        <v>11</v>
+      </c>
+      <c r="M7" t="n">
+        <v>13</v>
+      </c>
+      <c r="N7" t="n">
+        <v>74394.875</v>
+      </c>
+      <c r="O7" t="n">
+        <v>117009.625</v>
+      </c>
       <c r="P7" t="n">
-        <v>11</v>
+        <v>17923.84615384615</v>
       </c>
       <c r="Q7" t="n">
-        <v>13</v>
+        <v>28631.53846153846</v>
       </c>
       <c r="R7" t="n">
-        <v>74394.875</v>
+        <v>1859871.875</v>
       </c>
       <c r="S7" t="n">
-        <v>117009.625</v>
+        <v>209447.22875</v>
       </c>
       <c r="T7" t="n">
-        <v>17923.84615384615</v>
+        <v>25</v>
       </c>
       <c r="U7" t="n">
-        <v>28631.53846153846</v>
-      </c>
-      <c r="V7" t="n">
-        <v>1859871.875</v>
-      </c>
-      <c r="W7" t="n">
-        <v>209447.22875</v>
-      </c>
-      <c r="X7" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y7" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -1167,65 +977,37 @@
           <t>POLYGON ((476686.2248892394 4800294.277369834, 476671.3417148496 4799915.475286477, 476626.7839513996 4799539.00864393, 476552.8263123178 4799167.19848423, 476449.9247710427 4798802.337140651, 476318.7137497945 4798446.674104706, 476160.0022081513 4798102.402157281, 475974.7686555443 4797771.643849414, 475764.1551184215 4797456.43841606, 475529.4600992756 4797158.729203534, 475272.1305709437 4796880.351688129, 474993.7530555385 4796623.022159797, 474696.0438430125 4796388.327140652, 474380.8384096593 4796177.713603529, 474050.0801017919 4795992.480050921, 473705.8081543667 4795833.768509278, 473350.1451184215 4795702.55748803, 472985.283774843 4795599.655946755, 472613.4736151429 4795525.698307673, 472237.0069725954 4795481.140544224, 471858.2048892394 4795466.257369834, 471479.4028058834 4795481.140544224, 471102.9361633359 4795525.698307673, 470731.1260036358 4795599.655946755, 470366.2646600573 4795702.55748803, 470010.6016241121 4795833.768509278, 469666.3296766869 4795992.480050921, 469335.5713688195 4796177.713603529, 469020.3659354663 4796388.327140652, 468722.6567229403 4796623.022159797, 468444.2792075351 4796880.351688129, 468186.9496792032 4797158.729203534, 467952.2546600573 4797456.43841606, 467741.6411229345 4797771.643849414, 467556.4075703275 4798102.402157281, 467397.6960286843 4798446.674104706, 467266.4850074361 4798802.337140651, 467163.583466161 4799167.19848423, 467089.6258270792 4799539.00864393, 467045.0680636292 4799915.475286477, 467030.1848892394 4800294.277369834, 467045.0680636292 4800673.07945319, 467089.6258270792 4801049.546095737, 467163.583466161 4801421.356255437, 467266.4850074361 4801786.217599016, 467397.6960286843 4802141.880634961, 467556.4075703275 4802486.152582387, 467741.6411229345 4802816.910890253, 467952.2546600573 4803132.116323607, 468186.9496792032 4803429.825536133, 468444.2792075351 4803708.203051538, 468722.6567229403 4803965.53257987, 469020.3659354663 4804200.227599015, 469335.5713688195 4804410.841136138, 469666.3296766868 4804596.074688746, 470010.6016241121 4804754.786230389, 470366.2646600573 4804885.997251637, 470731.1260036358 4804988.898792912, 471102.9361633359 4805062.856431994, 471479.4028058834 4805107.414195444, 471858.2048892394 4805122.297369833, 472237.0069725953 4805107.414195444, 472613.4736151429 4805062.856431994, 472985.283774843 4804988.898792912, 473350.1451184215 4804885.997251637, 473705.8081543667 4804754.786230389, 474050.0801017919 4804596.074688746, 474380.8384096593 4804410.841136138, 474696.0438430125 4804200.227599015, 474993.7530555385 4803965.53257987, 475272.1305709436 4803708.203051538, 475529.4600992756 4803429.825536133, 475764.1551184215 4803132.116323607, 475974.7686555442 4802816.910890253, 476160.0022081513 4802486.152582387, 476318.7137497945 4802141.880634961, 476449.9247710427 4801786.217599016, 476552.8263123177 4801421.356255437, 476626.7839513995 4801049.546095737, 476671.3417148496 4800673.07945319, 476686.2248892394 4800294.277369834))</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 22 active permits
-20 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 8000 ft. 
-- The TVD for these well(s) are ~10000ft
-Devon has 21 permits, Grayson Mill Operating Llc has 1 permits</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>There are 2 wells within 3 mile radius that have started producing within last 4 years
-2.26 mi NW, Devon Energy Corporation has a H well at 10342 that has made 178 mbbl and 377 mmcf after 25 months of producing
-2.50 mi NW, Devon Energy Corporation has a H well at 10354 that has made 206 mbbl and 584 mmcf after 25 months of producing</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O8" s="2" t="n">
+      <c r="K8" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L8" t="n">
+        <v>22</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2</v>
+      </c>
+      <c r="N8" t="n">
+        <v>92678</v>
+      </c>
+      <c r="O8" t="n">
+        <v>190096</v>
+      </c>
       <c r="P8" t="n">
-        <v>22</v>
+        <v>22800</v>
       </c>
       <c r="Q8" t="n">
-        <v>2</v>
+        <v>45960</v>
       </c>
       <c r="R8" t="n">
-        <v>92678</v>
+        <v>2316950</v>
       </c>
       <c r="S8" t="n">
-        <v>190096</v>
+        <v>340271.84</v>
       </c>
       <c r="T8" t="n">
-        <v>22800</v>
+        <v>25</v>
       </c>
       <c r="U8" t="n">
-        <v>45960</v>
-      </c>
-      <c r="V8" t="n">
-        <v>2316950</v>
-      </c>
-      <c r="W8" t="n">
-        <v>340271.84</v>
-      </c>
-      <c r="X8" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y8" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -1272,65 +1054,37 @@
           <t>POLYGON ((475942.8275752033 4800429.924610612, 475927.9444008135 4800051.122527256, 475883.3866373634 4799674.655884708, 475809.4289982817 4799302.845725008, 475706.5274570066 4798937.98438143, 475575.3164357584 4798582.321345485, 475416.6048941152 4798238.049398059, 475231.3713415081 4797907.291090192, 475020.7578043854 4797592.085656838, 474786.0627852395 4797294.376444313, 474528.7332569076 4797015.998928907, 474250.3557415024 4796758.669400576, 473952.6465289763 4796523.97438143, 473637.4410956231 4796313.360844308, 473306.6827877558 4796128.1272917, 472962.4108403305 4795969.415750057, 472606.7478043854 4795838.204728808, 472241.8864608068 4795735.303187533, 471870.0763011068 4795661.345548452, 471493.6096585592 4795616.787785002, 471114.8075752032 4795601.904610612, 470736.0054918473 4795616.787785002, 470359.5388492997 4795661.345548452, 469987.7286895997 4795735.303187533, 469622.8673460211 4795838.204728808, 469267.204310076 4795969.415750057, 468922.9323626508 4796128.1272917, 468592.1740547834 4796313.360844308, 468276.9686214302 4796523.97438143, 467979.2594089042 4796758.669400576, 467700.881893499 4797015.998928907, 467443.552365167 4797294.376444313, 467208.8573460211 4797592.085656838, 466998.2438088984 4797907.291090192, 466813.0102562913 4798238.049398059, 466654.2987146481 4798582.321345485, 466523.0876933999 4798937.98438143, 466420.1861521248 4799302.845725008, 466346.2285130431 4799674.655884708, 466301.670749593 4800051.122527256, 466286.7875752032 4800429.924610612, 466301.670749593 4800808.726693968, 466346.2285130431 4801185.193336516, 466420.1861521248 4801557.003496216, 466523.0876933999 4801921.864839794, 466654.2987146481 4802277.527875739, 466813.0102562913 4802621.799823165, 466998.2438088984 4802952.558131032, 467208.8573460211 4803267.763564385, 467443.552365167 4803565.472776911, 467700.8818934989 4803843.850292317, 467979.2594089041 4804101.179820648, 468276.9686214301 4804335.874839794, 468592.1740547834 4804546.488376916, 468922.9323626507 4804731.721929524, 469267.2043100759 4804890.433471167, 469622.8673460211 4805021.644492416, 469987.7286895997 4805124.546033691, 470359.5388492997 4805198.503672772, 470736.0054918473 4805243.061436222, 471114.8075752032 4805257.944610612, 471493.6096585591 4805243.061436222, 471870.0763011068 4805198.503672772, 472241.8864608068 4805124.546033691, 472606.7478043853 4805021.644492416, 472962.4108403305 4804890.433471167, 473306.6827877557 4804731.721929524, 473637.4410956231 4804546.488376916, 473952.6465289763 4804335.874839794, 474250.3557415023 4804101.179820648, 474528.7332569075 4803843.850292317, 474786.0627852395 4803565.472776911, 475020.7578043853 4803267.763564385, 475231.3713415081 4802952.558131032, 475416.6048941151 4802621.799823165, 475575.3164357584 4802277.527875739, 475706.5274570066 4801921.864839794, 475809.4289982816 4801557.003496216, 475883.3866373634 4801185.193336516, 475927.9444008134 4800808.726693968, 475942.8275752033 4800429.924610612))</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 13 active permits
-11 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 8000 ft. 
-- The TVD for these well(s) are ~10100ft
-Devon has 13 permits</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>There are 2 wells within 3 mile radius that have started producing within last 4 years
-1.90 mi NW, Devon Energy Corporation has a H well at 10342 that has made 178 mbbl and 377 mmcf after 25 months of producing
-2.11 mi NW, Devon Energy Corporation has a H well at 10354 that has made 206 mbbl and 584 mmcf after 25 months of producing</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O9" s="2" t="n">
+      <c r="K9" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L9" t="n">
+        <v>13</v>
+      </c>
+      <c r="M9" t="n">
+        <v>2</v>
+      </c>
+      <c r="N9" t="n">
+        <v>92678</v>
+      </c>
+      <c r="O9" t="n">
+        <v>190096</v>
+      </c>
       <c r="P9" t="n">
-        <v>13</v>
+        <v>22800</v>
       </c>
       <c r="Q9" t="n">
-        <v>2</v>
+        <v>45960</v>
       </c>
       <c r="R9" t="n">
-        <v>92678</v>
+        <v>2316950</v>
       </c>
       <c r="S9" t="n">
-        <v>190096</v>
+        <v>340271.84</v>
       </c>
       <c r="T9" t="n">
-        <v>22800</v>
+        <v>25</v>
       </c>
       <c r="U9" t="n">
-        <v>45960</v>
-      </c>
-      <c r="V9" t="n">
-        <v>2316950</v>
-      </c>
-      <c r="W9" t="n">
-        <v>340271.84</v>
-      </c>
-      <c r="X9" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y9" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -1377,66 +1131,37 @@
           <t>POLYGON ((472430.5046453754 4799779.674300328, 472415.6214709856 4799400.872216972, 472371.0637075356 4799024.405574424, 472297.1060684538 4798652.595414724, 472194.2045271787 4798287.734071146, 472062.9935059305 4797932.071035201, 471904.2819642873 4797587.799087775, 471719.0484116803 4797257.040779908, 471508.4348745575 4796941.835346554, 471273.7398554116 4796644.126134029, 471016.4103270797 4796365.748618623, 470738.0328116745 4796108.419090291, 470440.3235991485 4795873.724071146, 470125.1181657953 4795663.110534023, 469794.3598579279 4795477.876981416, 469450.0879105027 4795319.165439772, 469094.4248745575 4795187.954418524, 468729.563530979 4795085.052877249, 468357.7533712789 4795011.095238168, 467981.2867287314 4794966.537474718, 467602.4846453754 4794951.654300328, 467223.6825620194 4794966.537474718, 466847.2159194719 4795011.095238168, 466475.4057597718 4795085.052877249, 466110.5444161933 4795187.954418524, 465754.8813802481 4795319.165439772, 465410.6094328229 4795477.876981416, 465079.8511249555 4795663.110534023, 464764.6456916023 4795873.724071146, 464466.9364790763 4796108.419090291, 464188.5589636712 4796365.748618623, 463931.2294353392 4796644.126134029, 463696.5344161933 4796941.835346554, 463485.9208790705 4797257.040779908, 463300.6873264635 4797587.799087775, 463141.9757848203 4797932.071035201, 463010.7647635721 4798287.734071146, 462907.863222297 4798652.595414724, 462833.9055832152 4799024.405574424, 462789.3478197652 4799400.872216972, 462774.4646453754 4799779.674300328, 462789.3478197652 4800158.476383684, 462833.9055832152 4800534.943026232, 462907.863222297 4800906.753185932, 463010.7647635721 4801271.61452951, 463141.9757848203 4801627.277565455, 463300.6873264635 4801971.549512881, 463485.9208790705 4802302.307820748, 463696.5344161933 4802617.513254101, 463931.2294353392 4802915.222466627, 464188.5589636711 4803193.599982033, 464466.9364790763 4803450.929510364, 464764.6456916023 4803685.62452951, 465079.8511249555 4803896.238066632, 465410.6094328229 4804081.47161924, 465754.8813802481 4804240.183160883, 466110.5444161933 4804371.394182132, 466475.4057597718 4804474.295723407, 466847.2159194719 4804548.253362488, 467223.6825620194 4804592.811125938, 467602.4846453754 4804607.694300327, 467981.2867287313 4804592.811125938, 468357.7533712789 4804548.253362488, 468729.563530979 4804474.295723407, 469094.4248745575 4804371.394182132, 469450.0879105027 4804240.183160883, 469794.3598579279 4804081.47161924, 470125.1181657953 4803896.238066632, 470440.3235991485 4803685.62452951, 470738.0328116745 4803450.929510364, 471016.4103270796 4803193.599982033, 471273.7398554116 4802915.222466627, 471508.4348745575 4802617.513254101, 471719.0484116802 4802302.307820748, 471904.2819642873 4801971.549512881, 472062.9935059305 4801627.277565455, 472194.2045271787 4801271.61452951, 472297.1060684538 4800906.753185932, 472371.0637075355 4800534.943026232, 472415.6214709856 4800158.476383684, 472430.5046453754 4799779.674300328))</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 21 active permits
-18 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 8000 ft. 
-- The TVD for these well(s) are ~9900ft
-Devon has 21 permits</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 15 wells within 3 mile radius that have started producing within last 4 years
-15 are H wells
-8 wells have produced for 2 to 3 months and have made between 22 to 85 mbbls with 20 to 92 mmcf of gas.  These wells are currently averaging 460 bpd and 723 mcfd.  3 wells have produced for 12 to 18 months and have made between 146 to 224 mbbls with 67 to 344 mmcf of gas.  These wells are currently averaging 81 bpd and 38 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-In 2014, Pacer Energy paid $3900/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O10" s="2" t="n">
+      <c r="K10" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L10" t="n">
+        <v>21</v>
+      </c>
+      <c r="M10" t="n">
+        <v>15</v>
+      </c>
+      <c r="N10" t="n">
+        <v>106735.4</v>
+      </c>
+      <c r="O10" t="n">
+        <v>155514.4</v>
+      </c>
       <c r="P10" t="n">
-        <v>21</v>
+        <v>23270</v>
       </c>
       <c r="Q10" t="n">
-        <v>15</v>
+        <v>28696</v>
       </c>
       <c r="R10" t="n">
-        <v>106735.4</v>
+        <v>2668385</v>
       </c>
       <c r="S10" t="n">
-        <v>155514.4</v>
+        <v>278370.776</v>
       </c>
       <c r="T10" t="n">
-        <v>23270</v>
+        <v>25</v>
       </c>
       <c r="U10" t="n">
-        <v>28696</v>
-      </c>
-      <c r="V10" t="n">
-        <v>2668385</v>
-      </c>
-      <c r="W10" t="n">
-        <v>278370.776</v>
-      </c>
-      <c r="X10" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y10" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -1483,66 +1208,37 @@
           <t>POLYGON ((470254.4470627511 4798968.314839863, 470239.5638883613 4798589.512756507, 470195.0061249112 4798213.04611396, 470121.0484858295 4797841.23595426, 470018.1469445544 4797476.374610681, 469886.9359233062 4797120.711574736, 469728.224381663 4796776.43962731, 469542.990829056 4796445.681319444, 469332.3772919332 4796130.47588609, 469097.6822727873 4795832.766673564, 468840.3527444554 4795554.389158159, 468561.9752290502 4795297.059629827, 468264.2660165242 4795062.364610681, 467949.060583171 4794851.751073559, 467618.3022753036 4794666.517520951, 467274.0303278784 4794507.805979308, 466918.3672919332 4794376.594958059, 466553.5059483547 4794273.693416785, 466181.6957886546 4794199.735777703, 465805.229146107 4794155.178014253, 465426.4270627511 4794140.294839864, 465047.6249793951 4794155.178014253, 464671.1583368476 4794199.735777703, 464299.3481771475 4794273.693416785, 463934.486833569 4794376.594958059, 463578.8237976238 4794507.805979308, 463234.5518501986 4794666.517520951, 462903.7935423312 4794851.751073559, 462588.588108978 4795062.364610681, 462290.878896452 4795297.059629827, 462012.5013810468 4795554.389158159, 461755.1718527148 4795832.766673564, 461520.4768335689 4796130.47588609, 461309.8632964463 4796445.681319444, 461124.6297438391 4796776.43962731, 460965.918202196 4797120.711574736, 460834.7071809478 4797476.374610681, 460731.8056396727 4797841.23595426, 460657.8480005909 4798213.04611396, 460613.2902371408 4798589.512756507, 460598.4070627511 4798968.314839863, 460613.2902371408 4799347.11692322, 460657.8480005909 4799723.583565767, 460731.8056396727 4800095.393725467, 460834.7071809478 4800460.255069045, 460965.918202196 4800815.91810499, 461124.6297438391 4801160.190052416, 461309.8632964462 4801490.948360283, 461520.4768335689 4801806.153793637, 461755.1718527148 4802103.863006162, 462012.5013810468 4802382.240521568, 462290.878896452 4802639.5700499, 462588.5881089779 4802874.265069045, 462903.7935423312 4803084.878606168, 463234.5518501985 4803270.112158775, 463578.8237976237 4803428.823700419, 463934.486833569 4803560.034721667, 464299.3481771475 4803662.936262942, 464671.1583368476 4803736.893902023, 465047.6249793951 4803781.451665473, 465426.4270627511 4803796.334839863, 465805.229146107 4803781.451665473, 466181.6957886546 4803736.893902023, 466553.5059483547 4803662.936262942, 466918.3672919332 4803560.034721667, 467274.0303278784 4803428.823700419, 467618.3022753036 4803270.112158775, 467949.060583171 4803084.878606168, 468264.2660165242 4802874.265069045, 468561.9752290501 4802639.5700499, 468840.3527444553 4802382.240521568, 469097.6822727873 4802103.863006162, 469332.3772919332 4801806.153793637, 469542.9908290559 4801490.948360283, 469728.224381663 4801160.190052416, 469886.9359233062 4800815.91810499, 470018.1469445544 4800460.255069045, 470121.0484858294 4800095.393725467, 470195.0061249112 4799723.583565767, 470239.5638883613 4799347.11692322, 470254.4470627511 4798968.314839863))</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 25 active permits
-22 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 8000 ft. 
-- The TVD for these well(s) are ~9900ft
-Devon has 25 permits</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 20 wells within 3 mile radius that have started producing within last 4 years
-20 are H wells
-8 wells have produced for 2 to 3 months and have made between 22 to 85 mbbls with 20 to 92 mmcf of gas.  These wells are currently averaging 460 bpd and 723 mcfd.  1 well has made 89 mbbl and 208 mmcfd in 8 months and is currently making 246 bpd and 753 mcfd.  1 well has made 176 mbbl and 252 mmcfd in 12 months and is currently making 332 bpd and 513 mcfd.  6 wells have produced for 12 to 18 months and have made between 146 to 224 mbbls with 67 to 344 mmcf of gas.  These wells are currently averaging 131 bpd and 121 mcfd.  2 wells have produced for 25 to 36 months and have made between 179 to 258 mbbls with 269 to 393 mmcf of gas.  These wells are currently averaging 87 bpd and 183 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-In 2014, Pacer Energy paid $3900/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O11" s="2" t="n">
+      <c r="K11" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L11" t="n">
+        <v>25</v>
+      </c>
+      <c r="M11" t="n">
+        <v>20</v>
+      </c>
+      <c r="N11" t="n">
+        <v>111610.6</v>
+      </c>
+      <c r="O11" t="n">
+        <v>147115.2</v>
+      </c>
       <c r="P11" t="n">
-        <v>25</v>
+        <v>25603.5</v>
       </c>
       <c r="Q11" t="n">
-        <v>20</v>
+        <v>30786</v>
       </c>
       <c r="R11" t="n">
-        <v>111610.6</v>
+        <v>2790265</v>
       </c>
       <c r="S11" t="n">
-        <v>147115.2</v>
+        <v>263336.208</v>
       </c>
       <c r="T11" t="n">
-        <v>25603.5</v>
+        <v>25</v>
       </c>
       <c r="U11" t="n">
-        <v>30786</v>
-      </c>
-      <c r="V11" t="n">
-        <v>2790265</v>
-      </c>
-      <c r="W11" t="n">
-        <v>263336.208</v>
-      </c>
-      <c r="X11" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y11" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -1589,66 +1285,37 @@
           <t>POLYGON ((471574.2336945967 4798869.261029639, 471559.350520207 4798490.458946283, 471514.7927567569 4798113.992303736, 471440.8351176751 4797742.182144036, 471337.9335764 4797377.320800457, 471206.7225551518 4797021.657764512, 471048.0110135087 4796677.385817086, 470862.7774609016 4796346.62750922, 470652.1639237789 4796031.422075866, 470417.468904633 4795733.71286334, 470160.139376301 4795455.335347935, 469881.7618608958 4795198.005819603, 469584.0526483698 4794963.310800457, 469268.8472150166 4794752.697263335, 468938.0889071493 4794567.463710727, 468593.816959724 4794408.752169084, 468238.1539237789 4794277.541147836, 467873.2925802003 4794174.639606561, 467501.4824205003 4794100.681967479, 467125.0157779527 4794056.124204029, 466746.2136945967 4794041.24102964, 466367.4116112408 4794056.124204029, 465990.9449686932 4794100.681967479, 465619.1348089931 4794174.639606561, 465254.2734654146 4794277.541147836, 464898.6104294694 4794408.752169084, 464554.3384820442 4794567.463710727, 464223.5801741768 4794752.697263335, 463908.3747408236 4794963.310800457, 463610.6655282977 4795198.005819603, 463332.2880128925 4795455.335347935, 463074.9584845605 4795733.71286334, 462840.2634654146 4796031.422075866, 462629.6499282919 4796346.62750922, 462444.4163756848 4796677.385817086, 462285.7048340416 4797021.657764512, 462154.4938127934 4797377.320800457, 462051.5922715183 4797742.182144036, 461977.6346324366 4798113.992303736, 461933.0768689865 4798490.458946283, 461918.1936945967 4798869.261029639, 461933.0768689865 4799248.063112996, 461977.6346324366 4799624.529755543, 462051.5922715183 4799996.339915243, 462154.4938127934 4800361.201258821, 462285.7048340416 4800716.864294766, 462444.4163756848 4801061.136242192, 462629.6499282919 4801391.894550059, 462840.2634654146 4801707.099983413, 463074.9584845605 4802004.809195939, 463332.2880128924 4802283.186711344, 463610.6655282976 4802540.516239676, 463908.3747408236 4802775.211258821, 464223.5801741768 4802985.824795944, 464554.3384820442 4803171.058348551, 464898.6104294694 4803329.769890195, 465254.2734654146 4803460.980911443, 465619.1348089931 4803563.882452718, 465990.9449686932 4803637.840091799, 466367.4116112408 4803682.397855249, 466746.2136945967 4803697.281029639, 467125.0157779526 4803682.397855249, 467501.4824205003 4803637.840091799, 467873.2925802003 4803563.882452718, 468238.1539237788 4803460.980911443, 468593.816959724 4803329.769890195, 468938.0889071492 4803171.058348551, 469268.8472150166 4802985.824795944, 469584.0526483698 4802775.211258821, 469881.7618608958 4802540.516239676, 470160.139376301 4802283.186711344, 470417.468904633 4802004.809195939, 470652.1639237788 4801707.099983413, 470862.7774609015 4801391.894550059, 471048.0110135086 4801061.136242192, 471206.7225551518 4800716.864294766, 471337.9335764 4800361.201258821, 471440.8351176751 4799996.339915243, 471514.7927567568 4799624.529755543, 471559.3505202069 4799248.063112996, 471574.2336945967 4798869.261029639))</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 22 active permits
-19 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 8000 ft. 
-- The TVD for these well(s) are ~10000ft
-Devon has 22 permits</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 16 wells within 3 mile radius that have started producing within last 4 years
-16 are H wells
-8 wells have produced for 2 to 3 months and have made between 22 to 85 mbbls with 20 to 92 mmcf of gas.  These wells are currently averaging 460 bpd and 723 mcfd.  1 well has made 176 mbbl and 252 mmcfd in 12 months and is currently making 332 bpd and 513 mcfd.  3 wells have produced for 12 to 18 months and have made between 146 to 224 mbbls with 67 to 344 mmcf of gas.  These wells are currently averaging 81 bpd and 38 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-In 2014, Pacer Energy paid $3900/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O12" s="2" t="n">
+      <c r="K12" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L12" t="n">
+        <v>22</v>
+      </c>
+      <c r="M12" t="n">
+        <v>16</v>
+      </c>
+      <c r="N12" t="n">
+        <v>106971.1666666667</v>
+      </c>
+      <c r="O12" t="n">
+        <v>153907.6666666667</v>
+      </c>
       <c r="P12" t="n">
-        <v>22</v>
+        <v>23651.25</v>
       </c>
       <c r="Q12" t="n">
-        <v>16</v>
+        <v>29206.875</v>
       </c>
       <c r="R12" t="n">
-        <v>106971.1666666667</v>
+        <v>2674279.166666667</v>
       </c>
       <c r="S12" t="n">
-        <v>153907.6666666667</v>
+        <v>275494.7233333333</v>
       </c>
       <c r="T12" t="n">
-        <v>23651.25</v>
+        <v>25</v>
       </c>
       <c r="U12" t="n">
-        <v>29206.875</v>
-      </c>
-      <c r="V12" t="n">
-        <v>2674279.166666667</v>
-      </c>
-      <c r="W12" t="n">
-        <v>275494.7233333333</v>
-      </c>
-      <c r="X12" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y12" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -1695,65 +1362,37 @@
           <t>POLYGON ((473099.9125895233 4799175.72778338, 473085.0294151335 4798796.925700024, 473040.4716516834 4798420.459057476, 472966.5140126017 4798048.648897776, 472863.6124713266 4797683.787554198, 472732.4014500784 4797328.124518253, 472573.6899084352 4796983.852570827, 472388.4563558282 4796653.09426296, 472177.8428187054 4796337.888829607, 471943.1477995595 4796040.179617081, 471685.8182712276 4795761.802101675, 471407.4407558224 4795504.472573344, 471109.7315432964 4795269.777554198, 470794.5261099432 4795059.164017076, 470463.7678020758 4794873.930464468, 470119.4958546506 4794715.218922825, 469763.8328187054 4794584.007901576, 469398.9714751269 4794481.106360301, 469027.1613154268 4794407.14872122, 468650.6946728792 4794362.59095777, 468271.8925895233 4794347.707783381, 467893.0905061673 4794362.59095777, 467516.6238636198 4794407.14872122, 467144.8137039197 4794481.106360301, 466779.9523603412 4794584.007901576, 466424.289324396 4794715.218922825, 466080.0173769708 4794873.930464468, 465749.2590691034 4795059.164017076, 465434.0536357502 4795269.777554198, 465136.3444232242 4795504.472573344, 464857.966907819 4795761.802101675, 464600.637379487 4796040.179617081, 464365.9423603411 4796337.888829607, 464155.3288232185 4796653.09426296, 463970.0952706113 4796983.852570827, 463811.3837289682 4797328.124518253, 463680.17270772 4797683.787554198, 463577.2711664449 4798048.648897776, 463503.3135273631 4798420.459057476, 463458.755763913 4798796.925700024, 463443.8725895233 4799175.72778338, 463458.755763913 4799554.529866736, 463503.3135273631 4799930.996509284, 463577.2711664449 4800302.806668984, 463680.17270772 4800667.668012562, 463811.3837289682 4801023.331048507, 463970.0952706113 4801367.602995933, 464155.3288232184 4801698.3613038, 464365.9423603411 4802013.566737154, 464600.637379487 4802311.275949679, 464857.966907819 4802589.653465085, 465136.3444232242 4802846.982993416, 465434.0536357501 4803081.678012562, 465749.2590691034 4803292.291549684, 466080.0173769707 4803477.525102292, 466424.2893243959 4803636.236643936, 466779.9523603412 4803767.447665184, 467144.8137039197 4803870.349206459, 467516.6238636198 4803944.30684554, 467893.0905061673 4803988.86460899, 468271.8925895233 4804003.74778338, 468650.6946728792 4803988.86460899, 469027.1613154268 4803944.30684554, 469398.9714751269 4803870.349206459, 469763.8328187054 4803767.447665184, 470119.4958546506 4803636.236643936, 470463.7678020758 4803477.525102292, 470794.5261099432 4803292.291549684, 471109.7315432964 4803081.678012562, 471407.4407558223 4802846.982993416, 471685.8182712275 4802589.653465085, 471943.1477995595 4802311.275949679, 472177.8428187054 4802013.566737154, 472388.4563558281 4801698.3613038, 472573.6899084352 4801367.602995933, 472732.4014500784 4801023.331048507, 472863.6124713266 4800667.668012562, 472966.5140126016 4800302.806668984, 473040.4716516834 4799930.996509284, 473085.0294151335 4799554.529866736, 473099.9125895233 4799175.72778338))</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 14 active permits
-11 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 7000 ft. 
-- The TVD for these well(s) are ~10500ft
-Devon has 14 permits</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 9 wells within 3 mile radius that have started producing within last 4 years
-9 are H wells
-5 wells have produced for 2 to 3 months and have made between 22 to 50 mbbls with 20 to 83 mmcf of gas.  These wells are currently averaging 424 bpd and 628 mcfd.  2 wells have produced for 12 to 18 months and have made between 178 to 224 mbbls with 67 to 344 mmcf of gas.  These wells are currently averaging 120 bpd and 56 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O13" s="2" t="n">
+      <c r="K13" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L13" t="n">
+        <v>14</v>
+      </c>
+      <c r="M13" t="n">
+        <v>9</v>
+      </c>
+      <c r="N13" t="n">
+        <v>108135.25</v>
+      </c>
+      <c r="O13" t="n">
+        <v>155151.5</v>
+      </c>
       <c r="P13" t="n">
-        <v>14</v>
+        <v>20966.66666666667</v>
       </c>
       <c r="Q13" t="n">
-        <v>9</v>
+        <v>28083.33333333333</v>
       </c>
       <c r="R13" t="n">
-        <v>108135.25</v>
+        <v>2703381.25</v>
       </c>
       <c r="S13" t="n">
-        <v>155151.5</v>
+        <v>277721.185</v>
       </c>
       <c r="T13" t="n">
-        <v>20966.66666666667</v>
+        <v>25</v>
       </c>
       <c r="U13" t="n">
-        <v>28083.33333333333</v>
-      </c>
-      <c r="V13" t="n">
-        <v>2703381.25</v>
-      </c>
-      <c r="W13" t="n">
-        <v>277721.185</v>
-      </c>
-      <c r="X13" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y13" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -1800,65 +1439,37 @@
           <t>POLYGON ((474720.78265296 4799196.952564376, 474705.8994785703 4798818.15048102, 474661.3417151202 4798441.683838473, 474587.3840760384 4798069.873678773, 474484.4825347633 4797705.012335194, 474353.2715135152 4797349.349299249, 474194.559971872 4797005.077351823, 474009.3264192649 4796674.319043957, 473798.7128821422 4796359.113610603, 473564.0178629963 4796061.404398077, 473306.6883346643 4795783.026882672, 473028.3108192591 4795525.69735434, 472730.6016067331 4795291.002335194, 472415.3961733799 4795080.388798072, 472084.6378655126 4794895.155245464, 471740.3659180873 4794736.443703821, 471384.7028821422 4794605.232682573, 471019.8415385636 4794502.331141298, 470648.0313788636 4794428.373502216, 470271.564736316 4794383.815738766, 469892.76265296 4794368.932564377, 469513.9605696041 4794383.815738766, 469137.4939270565 4794428.373502216, 468765.6837673564 4794502.331141298, 468400.8224237779 4794605.232682573, 468045.1593878327 4794736.443703821, 467700.8874404075 4794895.155245464, 467370.1291325401 4795080.388798072, 467054.9236991869 4795291.002335194, 466757.214486661 4795525.69735434, 466478.8369712558 4795783.026882672, 466221.5074429238 4796061.404398077, 465986.8124237779 4796359.113610603, 465776.1988866552 4796674.319043957, 465590.9653340481 4797005.077351823, 465432.2537924049 4797349.349299249, 465301.0427711567 4797705.012335194, 465198.1412298816 4798069.873678773, 465124.1835907999 4798441.683838473, 465079.6258273498 4798818.15048102, 465064.74265296 4799196.952564376, 465079.6258273498 4799575.754647733, 465124.1835907999 4799952.22129028, 465198.1412298816 4800324.03144998, 465301.0427711567 4800688.892793559, 465432.2537924049 4801044.555829504, 465590.9653340481 4801388.827776929, 465776.1988866552 4801719.586084796, 465986.8124237779 4802034.79151815, 466221.5074429238 4802332.500730676, 466478.8369712557 4802610.878246081, 466757.2144866609 4802868.207774413, 467054.9236991869 4803102.902793558, 467370.1291325401 4803313.516330681, 467700.8874404075 4803498.749883289, 468045.1593878327 4803657.461424932, 468400.8224237779 4803788.67244618, 468765.6837673564 4803891.573987455, 469137.4939270565 4803965.531626537, 469513.9605696041 4804010.089389986, 469892.76265296 4804024.972564376, 470271.5647363159 4804010.089389986, 470648.0313788636 4803965.531626537, 471019.8415385636 4803891.573987455, 471384.7028821421 4803788.67244618, 471740.3659180873 4803657.461424932, 472084.6378655125 4803498.749883289, 472415.3961733799 4803313.516330681, 472730.6016067331 4803102.902793558, 473028.3108192591 4802868.207774413, 473306.6883346643 4802610.878246081, 473564.0178629963 4802332.500730676, 473798.7128821421 4802034.79151815, 474009.3264192648 4801719.586084796, 474194.5599718719 4801388.827776929, 474353.2715135152 4801044.555829504, 474484.4825347633 4800688.892793559, 474587.3840760384 4800324.03144998, 474661.3417151201 4799952.22129028, 474705.8994785702 4799575.754647733, 474720.78265296 4799196.952564376))</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 10 active permits
-7 permits are H wells ; 2 permits are V wells 
-The average lateral length among these permits is 7000 ft. 
-- The TVD for these well(s) are ~10700ft
-Devon has 10 permits</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">There are 4 wells within 3 mile radius that have started producing within last 4 years
-4 are H wells
-2 wells have produced for 2 to 3 months and have made between 22 to 44 mbbls with 20 to 76 mmcf of gas.  These wells are currently averaging 364 bpd and 470 mcfd.  </t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  
-</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O14" s="2" t="n">
+      <c r="K14" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L14" t="n">
+        <v>10</v>
+      </c>
+      <c r="M14" t="n">
+        <v>4</v>
+      </c>
+      <c r="N14" t="n">
+        <v>92678</v>
+      </c>
+      <c r="O14" t="n">
+        <v>190096</v>
+      </c>
       <c r="P14" t="n">
-        <v>10</v>
+        <v>18975</v>
       </c>
       <c r="Q14" t="n">
-        <v>4</v>
+        <v>34620</v>
       </c>
       <c r="R14" t="n">
-        <v>92678</v>
+        <v>2316950</v>
       </c>
       <c r="S14" t="n">
-        <v>190096</v>
+        <v>340271.84</v>
       </c>
       <c r="T14" t="n">
-        <v>18975</v>
+        <v>25</v>
       </c>
       <c r="U14" t="n">
-        <v>34620</v>
-      </c>
-      <c r="V14" t="n">
-        <v>2316950</v>
-      </c>
-      <c r="W14" t="n">
-        <v>340271.84</v>
-      </c>
-      <c r="X14" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y14" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -1905,67 +1516,37 @@
           <t>POLYGON ((454633.1764049294 4793898.46923826, 454618.2932305396 4793519.667154904, 454573.7354670895 4793143.200512356, 454499.7778280078 4792771.390352656, 454396.8762867327 4792406.529009078, 454265.6652654845 4792050.865973133, 454106.9537238413 4791706.594025707, 453921.7201712342 4791375.83571784, 453711.1066341115 4791060.630284486, 453476.4116149656 4790762.921071961, 453219.0820866337 4790484.543556555, 452940.7045712285 4790227.214028223, 452642.9953587024 4789992.519009078, 452327.7899253492 4789781.905471955, 451997.0316174819 4789596.671919348, 451652.7596700566 4789437.960377704, 451297.0966341115 4789306.749356456, 450932.2352905329 4789203.847815181, 450560.4251308329 4789129.8901761, 450183.9584882853 4789085.33241265, 449805.1564049294 4789070.44923826, 449426.3543215734 4789085.33241265, 449049.8876790258 4789129.8901761, 448678.0775193258 4789203.847815181, 448313.2161757472 4789306.749356456, 447957.5531398021 4789437.960377704, 447613.2811923769 4789596.671919348, 447282.5228845095 4789781.905471955, 446967.3174511563 4789992.519009078, 446669.6082386303 4790227.214028223, 446391.2307232251 4790484.543556555, 446133.9011948931 4790762.921071961, 445899.2061757472 4791060.630284486, 445688.5926386245 4791375.83571784, 445503.3590860174 4791706.594025707, 445344.6475443742 4792050.865973133, 445213.436523126 4792406.529009078, 445110.5349818509 4792771.390352656, 445036.5773427692 4793143.200512356, 444992.0195793191 4793519.667154904, 444977.1364049293 4793898.46923826, 444992.0195793191 4794277.271321616, 445036.5773427692 4794653.737964164, 445110.5349818509 4795025.548123864, 445213.436523126 4795390.409467442, 445344.6475443742 4795746.072503387, 445503.3590860174 4796090.344450813, 445688.5926386245 4796421.10275868, 445899.2061757472 4796736.308192033, 446133.9011948931 4797034.017404559, 446391.230723225 4797312.394919964, 446669.6082386302 4797569.724448296, 446967.3174511562 4797804.419467442, 447282.5228845095 4798015.033004564, 447613.2811923768 4798200.266557172, 447957.553139802 4798358.978098815, 448313.2161757472 4798490.189120064, 448678.0775193258 4798593.090661339, 449049.8876790258 4798667.04830042, 449426.3543215734 4798711.60606387, 449805.1564049294 4798726.489238259, 450183.9584882853 4798711.60606387, 450560.4251308329 4798667.04830042, 450932.2352905329 4798593.090661339, 451297.0966341114 4798490.189120064, 451652.7596700566 4798358.978098815, 451997.0316174818 4798200.266557172, 452327.7899253492 4798015.033004564, 452642.9953587024 4797804.419467442, 452940.7045712284 4797569.724448296, 453219.0820866336 4797312.394919964, 453476.4116149656 4797034.017404559, 453711.1066341114 4796736.308192033, 453921.7201712342 4796421.10275868, 454106.9537238412 4796090.344450813, 454265.6652654845 4795746.072503387, 454396.8762867327 4795390.409467442, 454499.7778280077 4795025.548123864, 454573.7354670895 4794653.737964164, 454618.2932305395 4794277.271321616, 454633.1764049294 4793898.46923826))</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 36 active permits
-23 permits are H wells ; 13 permits are V wells 
-The average lateral length among these permits is 10000 ft. 
-- The TVD for these well(s) are ~11600ft
-Elephant Operating Llc has 31 permits, Eog Resources has 3 permits, Eog Resources Inc has 2 permits</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>There are 2 wells within 3 mile radius that have started producing within last 4 years
-2.49 mi NE, Eog Resources Incorporated has a H well at 11855 that has made 42 mbbl and 177 mmcf after 8 months of producing
-2.50 mi NE, Eog Resources Incorporated has a H well at 11855 that has made 49 mbbl and 209 mmcf after 8 months of producing</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Samson Resources paid $1526/acre.  The weighted average price in 2019 overall within the 3 radius was $1569/acre.  The highest price paid in 2019 was $5751/acre
-In 2018, Contex Energy paid $4002/acre. 
-In 2016, Hoover &amp; Stacy paid $750/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O15" s="2" t="n">
+      <c r="K15" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L15" t="n">
+        <v>36</v>
+      </c>
+      <c r="M15" t="n">
+        <v>2</v>
+      </c>
+      <c r="N15" t="n">
+        <v>38988</v>
+      </c>
+      <c r="O15" t="n">
+        <v>170744</v>
+      </c>
       <c r="P15" t="n">
-        <v>36</v>
+        <v>9225</v>
       </c>
       <c r="Q15" t="n">
-        <v>2</v>
+        <v>40440</v>
       </c>
       <c r="R15" t="n">
-        <v>38988</v>
+        <v>974700</v>
       </c>
       <c r="S15" t="n">
-        <v>170744</v>
+        <v>305631.76</v>
       </c>
       <c r="T15" t="n">
-        <v>9225</v>
+        <v>25</v>
       </c>
       <c r="U15" t="n">
-        <v>40440</v>
-      </c>
-      <c r="V15" t="n">
-        <v>974700</v>
-      </c>
-      <c r="W15" t="n">
-        <v>305631.76</v>
-      </c>
-      <c r="X15" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y15" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -2012,66 +1593,37 @@
           <t>POLYGON ((453633.3525036267 4793919.754942623, 453618.4693292369 4793540.952859267, 453573.9115657868 4793164.486216719, 453499.9539267051 4792792.676057019, 453397.05238543 4792427.814713441, 453265.8413641818 4792072.151677496, 453107.1298225386 4791727.87973007, 452921.8962699315 4791397.121422203, 452711.2827328088 4791081.915988849, 452476.5877136629 4790784.206776324, 452219.258185331 4790505.829260918, 451940.8806699258 4790248.499732587, 451643.1714573997 4790013.804713441, 451327.9660240465 4789803.191176319, 450997.2077161792 4789617.957623711, 450652.9357687539 4789459.246082067, 450297.2727328088 4789328.035060819, 449932.4113892302 4789225.133519544, 449560.6012295302 4789151.175880463, 449184.1345869826 4789106.618117013, 448805.3325036266 4789091.734942623, 448426.5304202707 4789106.618117013, 448050.0637777231 4789151.175880463, 447678.2536180231 4789225.133519544, 447313.3922744445 4789328.035060819, 446957.7292384994 4789459.246082067, 446613.4572910742 4789617.957623711, 446282.6989832068 4789803.191176319, 445967.4935498536 4790013.804713441, 445669.7843373276 4790248.499732587, 445391.4068219224 4790505.829260918, 445134.0772935904 4790784.206776324, 444899.3822744445 4791081.915988849, 444688.7687373218 4791397.121422203, 444503.5351847147 4791727.87973007, 444344.8236430715 4792072.151677496, 444213.6126218233 4792427.814713441, 444110.7110805482 4792792.676057019, 444036.7534414665 4793164.486216719, 443992.1956780164 4793540.952859267, 443977.3125036266 4793919.754942623, 443992.1956780164 4794298.557025979, 444036.7534414665 4794675.023668527, 444110.7110805482 4795046.833828227, 444213.6126218233 4795411.695171805, 444344.8236430715 4795767.35820775, 444503.5351847147 4796111.630155176, 444688.7687373218 4796442.388463043, 444899.3822744445 4796757.593896396, 445134.0772935904 4797055.303108922, 445391.4068219223 4797333.680624328, 445669.7843373275 4797591.010152659, 445967.4935498535 4797825.705171805, 446282.6989832068 4798036.318708927, 446613.4572910741 4798221.552261535, 446957.7292384993 4798380.263803178, 447313.3922744445 4798511.474824427, 447678.2536180231 4798614.376365702, 448050.0637777231 4798688.334004783, 448426.5304202707 4798732.891768233, 448805.3325036266 4798747.774942623, 449184.1345869825 4798732.891768233, 449560.6012295302 4798688.334004783, 449932.4113892302 4798614.376365702, 450297.2727328087 4798511.474824427, 450652.9357687539 4798380.263803178, 450997.2077161791 4798221.552261535, 451327.9660240465 4798036.318708927, 451643.1714573997 4797825.705171805, 451940.8806699257 4797591.010152659, 452219.2581853309 4797333.680624328, 452476.5877136629 4797055.303108922, 452711.2827328087 4796757.593896396, 452921.8962699315 4796442.388463043, 453107.1298225385 4796111.630155176, 453265.8413641818 4795767.35820775, 453397.05238543 4795411.695171805, 453499.953926705 4795046.833828227, 453573.9115657868 4794675.023668527, 453618.4693292368 4794298.557025979, 453633.3525036267 4793919.754942623))</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 21 active permits
-15 permits are H wells ; 6 permits are V wells 
-The average lateral length among these permits is 10000 ft. 
-- The TVD for these well(s) are ~11400ft
-Elephant Operating Llc has 16 permits, Eog Resources has 3 permits, Eog Resources Inc has 2 permits</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>There are 2 wells within 3 mile radius that have started producing within last 4 years
-2.67 mi NE, Eog Resources Incorporated has a H well at 11855 that has made 42 mbbl and 177 mmcf after 8 months of producing
-2.68 mi NE, Eog Resources Incorporated has a H well at 11855 that has made 49 mbbl and 209 mmcf after 8 months of producing</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Titan Expl paid $5751/acre.  The weighted average price in 2019 overall within the 3 radius was $1569/acre.  The highest price paid in 2019 was $5751/acre
-In 2018, Contex Energy paid $4002/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O16" s="2" t="n">
+      <c r="K16" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L16" t="n">
+        <v>21</v>
+      </c>
+      <c r="M16" t="n">
+        <v>2</v>
+      </c>
+      <c r="N16" t="n">
+        <v>38988</v>
+      </c>
+      <c r="O16" t="n">
+        <v>170744</v>
+      </c>
       <c r="P16" t="n">
-        <v>21</v>
+        <v>9225</v>
       </c>
       <c r="Q16" t="n">
-        <v>2</v>
+        <v>40440</v>
       </c>
       <c r="R16" t="n">
-        <v>38988</v>
+        <v>974700</v>
       </c>
       <c r="S16" t="n">
-        <v>170744</v>
+        <v>305631.76</v>
       </c>
       <c r="T16" t="n">
-        <v>9225</v>
+        <v>25</v>
       </c>
       <c r="U16" t="n">
-        <v>40440</v>
-      </c>
-      <c r="V16" t="n">
-        <v>974700</v>
-      </c>
-      <c r="W16" t="n">
-        <v>305631.76</v>
-      </c>
-      <c r="X16" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y16" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -2118,38 +1670,23 @@
           <t>POLYGON ((452522.6375132183 4793446.594994583, 452507.7543388285 4793067.792911227, 452463.1965753784 4792691.326268679, 452389.2389362967 4792319.516108979, 452286.3373950216 4791954.654765401, 452155.1263737734 4791598.991729456, 451996.4148321302 4791254.71978203, 451811.1812795231 4790923.961474163, 451600.5677424004 4790608.75604081, 451365.8727232545 4790311.046828284, 451108.5431949226 4790032.669312879, 450830.1656795174 4789775.339784547, 450532.4564669913 4789540.644765401, 450217.2510336381 4789330.031228279, 449886.4927257708 4789144.797675671, 449542.2207783455 4788986.086134028, 449186.5577424004 4788854.875112779, 448821.6963988218 4788751.973571504, 448449.8862391218 4788678.015932423, 448073.4195965742 4788633.458168973, 447694.6175132183 4788618.574994584, 447315.8154298623 4788633.458168973, 446939.3487873147 4788678.015932423, 446567.5386276147 4788751.973571504, 446202.6772840361 4788854.875112779, 445847.014248091 4788986.086134028, 445502.7423006658 4789144.797675671, 445171.9839927984 4789330.031228279, 444856.7785594452 4789540.644765401, 444559.0693469192 4789775.339784547, 444280.691831514 4790032.669312879, 444023.362303182 4790311.046828284, 443788.6672840361 4790608.75604081, 443578.0537469134 4790923.961474163, 443392.8201943063 4791254.71978203, 443234.1086526631 4791598.991729456, 443102.8976314149 4791954.654765401, 442999.9960901398 4792319.516108979, 442926.0384510581 4792691.326268679, 442881.480687608 4793067.792911227, 442866.5975132182 4793446.594994583, 442881.480687608 4793825.397077939, 442926.0384510581 4794201.863720487, 442999.9960901398 4794573.673880187, 443102.8976314149 4794938.535223765, 443234.1086526631 4795294.19825971, 443392.8201943063 4795638.470207136, 443578.0537469134 4795969.228515003, 443788.6672840361 4796284.433948357, 444023.362303182 4796582.143160882, 444280.6918315139 4796860.520676288, 444559.0693469191 4797117.85020462, 444856.7785594451 4797352.545223765, 445171.9839927984 4797563.158760888, 445502.7423006657 4797748.392313495, 445847.0142480909 4797907.103855139, 446202.6772840361 4798038.314876387, 446567.5386276147 4798141.216417662, 446939.3487873147 4798215.174056743, 447315.8154298623 4798259.731820193, 447694.6175132183 4798274.614994583, 448073.4195965742 4798259.731820193, 448449.8862391218 4798215.174056743, 448821.6963988218 4798141.216417662, 449186.5577424003 4798038.314876387, 449542.2207783455 4797907.103855139, 449886.4927257707 4797748.392313495, 450217.2510336381 4797563.158760888, 450532.4564669913 4797352.545223765, 450830.1656795173 4797117.85020462, 451108.5431949225 4796860.520676288, 451365.8727232545 4796582.143160882, 451600.5677424003 4796284.433948357, 451811.1812795231 4795969.228515003, 451996.4148321301 4795638.470207136, 452155.1263737734 4795294.19825971, 452286.3373950216 4794938.535223765, 452389.2389362966 4794573.673880187, 452463.1965753784 4794201.863720487, 452507.7543388284 4793825.397077939, 452522.6375132183 4793446.594994583))</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 18 active permits
-12 permits are H wells ; 6 permits are V wells 
-The average lateral length among these permits is 10000 ft. 
-- The TVD for these well(s) are ~11300ft
-Elephant Operating Llc has 16 permits, Eog Resources Inc has 2 permits</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>There are no new wells in the last 4 years within a 3 mile radius</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Titan Expl paid $5751/acre.  The weighted average price in 2019 overall within the 3 radius was $1569/acre.  The highest price paid in 2019 was $5751/acre
-In 2018, Contex Energy paid $4002/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O17" s="2" t="n">
+      <c r="K17" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L17" t="n">
+        <v>18</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
       <c r="P17" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
@@ -2161,21 +1698,9 @@
         <v>0</v>
       </c>
       <c r="T17" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="U17" t="n">
-        <v>0</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0</v>
-      </c>
-      <c r="W17" t="n">
-        <v>0</v>
-      </c>
-      <c r="X17" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y17" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -2222,38 +1747,23 @@
           <t>POLYGON ((451679.1672105166 4792477.806125961, 451664.2840361268 4792099.004042605, 451619.7262726767 4791722.537400058, 451545.768633595 4791350.727240358, 451442.8670923199 4790985.865896779, 451311.6560710717 4790630.202860834, 451152.9445294285 4790285.930913408, 450967.7109768214 4789955.172605542, 450757.0974396987 4789639.967172188, 450522.4024205528 4789342.257959662, 450265.0728922209 4789063.880444257, 449986.6953768157 4788806.550915925, 449688.9861642896 4788571.855896779, 449373.7807309364 4788361.242359657, 449043.0224230691 4788176.008807049, 448698.7504756438 4788017.297265406, 448343.0874396987 4787886.086244158, 447978.2260961201 4787783.184702883, 447606.4159364201 4787709.227063801, 447229.9492938725 4787664.669300351, 446851.1472105166 4787649.786125962, 446472.3451271606 4787664.669300351, 446095.878484613 4787709.227063801, 445724.068324913 4787783.184702883, 445359.2069813344 4787886.086244158, 445003.5439453893 4788017.297265406, 444659.2719979641 4788176.008807049, 444328.5136900967 4788361.242359657, 444013.3082567435 4788571.855896779, 443715.5990442175 4788806.550915925, 443437.2215288123 4789063.880444257, 443179.8920004803 4789342.257959662, 442945.1969813344 4789639.967172188, 442734.5834442117 4789955.172605542, 442549.3498916046 4790285.930913408, 442390.6383499614 4790630.202860834, 442259.4273287132 4790985.865896779, 442156.5257874381 4791350.727240358, 442082.5681483564 4791722.537400058, 442038.0103849063 4792099.004042605, 442023.1272105165 4792477.806125961, 442038.0103849063 4792856.608209318, 442082.5681483564 4793233.074851865, 442156.5257874381 4793604.885011565, 442259.4273287132 4793969.746355143, 442390.6383499614 4794325.409391088, 442549.3498916046 4794669.681338514, 442734.5834442117 4795000.439646381, 442945.1969813344 4795315.645079735, 443179.8920004803 4795613.35429226, 443437.2215288123 4795891.731807666, 443715.5990442174 4796149.061335998, 444013.3082567434 4796383.756355143, 444328.5136900967 4796594.369892266, 444659.271997964 4796779.603444873, 445003.5439453892 4796938.314986517, 445359.2069813344 4797069.526007765, 445724.068324913 4797172.42754904, 446095.878484613 4797246.385188121, 446472.3451271606 4797290.942951571, 446851.1472105166 4797305.826125961, 447229.9492938725 4797290.942951571, 447606.4159364201 4797246.385188121, 447978.2260961201 4797172.42754904, 448343.0874396986 4797069.526007765, 448698.7504756438 4796938.314986517, 449043.0224230691 4796779.603444873, 449373.7807309364 4796594.369892266, 449688.9861642896 4796383.756355143, 449986.6953768156 4796149.061335998, 450265.0728922208 4795891.731807666, 450522.4024205528 4795613.35429226, 450757.0974396986 4795315.645079735, 450967.7109768214 4795000.439646381, 451152.9445294284 4794669.681338514, 451311.6560710717 4794325.409391088, 451442.8670923199 4793969.746355143, 451545.7686335949 4793604.885011565, 451619.7262726767 4793233.074851865, 451664.2840361267 4792856.608209318, 451679.1672105166 4792477.806125961))</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 9 active permits
-9 permits are H wells 
-The average lateral length among these permits is 10000 ft. 
-- The TVD for these well(s) are ~12000ft
-Elephant Operating Llc has 4 permits, Eog Resources Inc has 2 permits, Wold Energy Partners has 1 permits</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>There are no new wells in the last 4 years within a 3 mile radius</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Titan Expl paid $5751/acre.  2323 Ss paid $302/acre.  The weighted average price in 2019 overall within the 3 radius was $1575/acre.  The highest price paid in 2019 was $5751/acre
-In 2018, Contex Energy paid $4002/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O18" s="2" t="n">
+      <c r="K18" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L18" t="n">
+        <v>9</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
       <c r="P18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="n">
         <v>0</v>
@@ -2265,21 +1775,9 @@
         <v>0</v>
       </c>
       <c r="T18" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="U18" t="n">
-        <v>0</v>
-      </c>
-      <c r="V18" t="n">
-        <v>0</v>
-      </c>
-      <c r="W18" t="n">
-        <v>0</v>
-      </c>
-      <c r="X18" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y18" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -2326,66 +1824,37 @@
           <t>POLYGON ((449808.5861090592 4789952.455238507, 449793.7029346694 4789573.653155151, 449749.1451712193 4789197.186512603, 449675.1875321376 4788825.376352903, 449572.2859908625 4788460.515009325, 449441.0749696143 4788104.85197338, 449282.3634279711 4787760.580025954, 449097.129875364 4787429.821718087, 448886.5163382413 4787114.616284734, 448651.8213190954 4786816.907072208, 448394.4917907635 4786538.529556802, 448116.1142753583 4786281.200028471, 447818.4050628322 4786046.505009325, 447503.199629479 4785835.891472203, 447172.4413216117 4785650.657919595, 446828.1693741864 4785491.946377952, 446472.5063382413 4785360.735356703, 446107.6449946627 4785257.833815428, 445735.8348349627 4785183.876176347, 445359.3681924151 4785139.318412897, 444980.5661090591 4785124.435238508, 444601.7640257032 4785139.318412897, 444225.2973831556 4785183.876176347, 443853.4872234556 4785257.833815428, 443488.625879877 4785360.735356703, 443132.9628439319 4785491.946377952, 442788.6908965067 4785650.657919595, 442457.9325886393 4785835.891472203, 442142.7271552861 4786046.505009325, 441845.0179427601 4786281.200028471, 441566.6404273549 4786538.529556802, 441309.3108990229 4786816.907072208, 441074.615879877 4787114.616284734, 440864.0023427543 4787429.821718087, 440678.7687901472 4787760.580025954, 440520.057248504 4788104.85197338, 440388.8462272558 4788460.515009325, 440285.9446859807 4788825.376352903, 440211.987046899 4789197.186512603, 440167.4292834489 4789573.653155151, 440152.5461090591 4789952.455238507, 440167.4292834489 4790331.257321863, 440211.987046899 4790707.723964411, 440285.9446859807 4791079.534124111, 440388.8462272558 4791444.395467689, 440520.057248504 4791800.058503634, 440678.7687901472 4792144.33045106, 440864.0023427543 4792475.088758927, 441074.615879877 4792790.294192281, 441309.3108990229 4793088.003404806, 441566.6404273548 4793366.380920212, 441845.01794276 4793623.710448544, 442142.727155286 4793858.405467689, 442457.9325886393 4794069.019004812, 442788.6908965066 4794254.252557419, 443132.9628439318 4794412.964099063, 443488.625879877 4794544.175120311, 443853.4872234556 4794647.076661586, 444225.2973831556 4794721.034300667, 444601.7640257032 4794765.592064117, 444980.5661090591 4794780.475238507, 445359.368192415 4794765.592064117, 445735.8348349627 4794721.034300667, 446107.6449946627 4794647.076661586, 446472.5063382412 4794544.175120311, 446828.1693741864 4794412.964099063, 447172.4413216116 4794254.252557419, 447503.199629479 4794069.019004812, 447818.4050628322 4793858.405467689, 448116.1142753582 4793623.710448544, 448394.4917907634 4793366.380920212, 448651.8213190954 4793088.003404806, 448886.5163382412 4792790.294192281, 449097.129875364 4792475.088758927, 449282.363427971 4792144.33045106, 449441.0749696143 4791800.058503634, 449572.2859908625 4791444.395467689, 449675.1875321375 4791079.534124111, 449749.1451712193 4790707.723964411, 449793.7029346693 4790331.257321863, 449808.5861090592 4789952.455238507))</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 4 active permits
-4 permits are H wells 
-The average lateral length among these permits is 10000 ft. 
-- The TVD for these well(s) are ~12400ft
-Wold Energy Partners has 2 permits, Wold Energy Partners Llc has 2 permits</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>There are 2 wells within 3 mile radius that have started producing within last 4 years
-1.91 mi SW, Wold Energy Partners Llc has a H well at 11014 that has made 233 mbbl and 187 mmcf after 38 months of producing
-1.88 mi SW, Wold Energy Partners Llc has a H well at 12577 that has made 486 mbbl and 1589 mmcf after 19 months of producing</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2013.
-Lone Tree Energy paid $570/acre.  
-In 2010, Southwestern Prod paid $700/acre. 
-</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O19" s="2" t="n">
+      <c r="K19" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L19" t="n">
+        <v>4</v>
+      </c>
+      <c r="M19" t="n">
+        <v>2</v>
+      </c>
+      <c r="N19" t="n">
+        <v>188394</v>
+      </c>
+      <c r="O19" t="n">
+        <v>422507.5</v>
+      </c>
       <c r="P19" t="n">
-        <v>4</v>
+        <v>50955</v>
       </c>
       <c r="Q19" t="n">
-        <v>2</v>
+        <v>97095</v>
       </c>
       <c r="R19" t="n">
-        <v>188394</v>
+        <v>4709850</v>
       </c>
       <c r="S19" t="n">
-        <v>422507.5</v>
+        <v>756288.425</v>
       </c>
       <c r="T19" t="n">
-        <v>50955</v>
+        <v>25</v>
       </c>
       <c r="U19" t="n">
-        <v>97095</v>
-      </c>
-      <c r="V19" t="n">
-        <v>4709850</v>
-      </c>
-      <c r="W19" t="n">
-        <v>756288.425</v>
-      </c>
-      <c r="X19" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y19" t="n">
         <v>1.79</v>
       </c>
     </row>
@@ -2432,65 +1901,37 @@
           <t>POLYGON ((450599.1527411023 4790347.606312461, 450584.2695667125 4789968.804229105, 450539.7118032624 4789592.337586557, 450465.7541641807 4789220.527426858, 450362.8526229056 4788855.666083279, 450231.6416016574 4788500.003047334, 450072.9300600142 4788155.731099908, 449887.6965074071 4787824.972792041, 449677.0829702844 4787509.767358688, 449442.3879511385 4787212.058146162, 449185.0584228066 4786933.680630757, 448906.6809074014 4786676.351102425, 448608.9716948753 4786441.656083279, 448293.7662615221 4786231.042546157, 447963.0079536548 4786045.808993549, 447618.7360062295 4785887.097451906, 447263.0729702844 4785755.886430657, 446898.2116267058 4785652.984889382, 446526.4014670058 4785579.027250301, 446149.9348244582 4785534.469486851, 445771.1327411023 4785519.586312462, 445392.3306577463 4785534.469486851, 445015.8640151987 4785579.027250301, 444644.0538554987 4785652.984889382, 444279.1925119201 4785755.886430657, 443923.529475975 4785887.097451906, 443579.2575285498 4786045.808993549, 443248.4992206824 4786231.042546157, 442933.2937873292 4786441.656083279, 442635.5845748032 4786676.351102425, 442357.207059398 4786933.680630757, 442099.877531066 4787212.058146162, 441865.1825119201 4787509.767358688, 441654.5689747974 4787824.972792041, 441469.3354221903 4788155.731099908, 441310.6238805471 4788500.003047334, 441179.4128592989 4788855.666083279, 441076.5113180238 4789220.527426858, 441002.5536789421 4789592.337586557, 440957.995915492 4789968.804229105, 440943.1127411022 4790347.606312461, 440957.995915492 4790726.408395818, 441002.5536789421 4791102.875038365, 441076.5113180238 4791474.685198065, 441179.4128592989 4791839.546541643, 441310.6238805471 4792195.209577588, 441469.3354221903 4792539.481525014, 441654.5689747974 4792870.239832881, 441865.1825119201 4793185.445266235, 442099.877531066 4793483.15447876, 442357.2070593979 4793761.531994166, 442635.5845748031 4794018.861522498, 442933.2937873291 4794253.556541643, 443248.4992206824 4794464.170078766, 443579.2575285497 4794649.403631373, 443923.5294759749 4794808.115173017, 444279.1925119201 4794939.326194265, 444644.0538554987 4795042.22773554, 445015.8640151987 4795116.185374621, 445392.3306577463 4795160.743138071, 445771.1327411023 4795175.626312461, 446149.9348244581 4795160.743138071, 446526.4014670058 4795116.185374621, 446898.2116267058 4795042.22773554, 447263.0729702843 4794939.326194265, 447618.7360062295 4794808.115173017, 447963.0079536547 4794649.403631373, 448293.7662615221 4794464.170078766, 448608.9716948753 4794253.556541643, 448906.6809074013 4794018.861522498, 449185.0584228065 4793761.531994166, 449442.3879511385 4793483.15447876, 449677.0829702843 4793185.445266235, 449887.6965074071 4792870.239832881, 450072.9300600141 4792539.481525014, 450231.6416016574 4792195.209577588, 450362.8526229056 4791839.546541643, 450465.7541641806 4791474.685198065, 450539.7118032624 4791102.875038365, 450584.2695667124 4790726.408395818, 450599.1527411023 4790347.606312461))</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>In a 3 mile radius there are 7 active permits
-7 permits are H wells 
-The average lateral length among these permits is 10000 ft. 
-- The TVD for these well(s) are ~12000ft
-Elephant Operating Llc has 3 permits, Eog Resources Inc has 1 permits, Wold Energy Partners has 1 permits</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>There are 2 wells within 3 mile radius that have started producing within last 4 years
-2.45 mi SW, Wold Energy Partners Llc has a H well at 11014 that has made 233 mbbl and 187 mmcf after 38 months of producing
-2.42 mi SW, Wold Energy Partners Llc has a H well at 12577 that has made 486 mbbl and 1589 mmcf after 19 months of producing</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2010.
-Southwestern Prod paid $700/acre.  
-</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>No old wells within tract or in 3 mile radius of tract.</t>
-        </is>
-      </c>
-      <c r="O20" s="2" t="n">
+      <c r="K20" s="2" t="n">
         <v>43913</v>
       </c>
+      <c r="L20" t="n">
+        <v>7</v>
+      </c>
+      <c r="M20" t="n">
+        <v>2</v>
+      </c>
+      <c r="N20" t="n">
+        <v>188394</v>
+      </c>
+      <c r="O20" t="n">
+        <v>422507.5</v>
+      </c>
       <c r="P20" t="n">
-        <v>7</v>
+        <v>50955</v>
       </c>
       <c r="Q20" t="n">
-        <v>2</v>
+        <v>97095</v>
       </c>
       <c r="R20" t="n">
-        <v>188394</v>
+        <v>4709850</v>
       </c>
       <c r="S20" t="n">
-        <v>422507.5</v>
+        <v>756288.425</v>
       </c>
       <c r="T20" t="n">
-        <v>50955</v>
+        <v>25</v>
       </c>
       <c r="U20" t="n">
-        <v>97095</v>
-      </c>
-      <c r="V20" t="n">
-        <v>4709850</v>
-      </c>
-      <c r="W20" t="n">
-        <v>756288.425</v>
-      </c>
-      <c r="X20" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y20" t="n">
         <v>1.79</v>
       </c>
     </row>

</xml_diff>